<commit_message>
update: add "Numéro de lot des logements" in edd_files instead of type
</commit_message>
<xml_diff>
--- a/static/files/logements_edd.xlsx
+++ b/static/files/logements_edd.xlsx
@@ -30,7 +30,7 @@
     <t xml:space="preserve">Désignation des logements</t>
   </si>
   <si>
-    <t xml:space="preserve">N° de lot des logements</t>
+    <t xml:space="preserve">Numéro de lot des logements</t>
   </si>
   <si>
     <t xml:space="preserve">(choisir dans la liste déroulante)</t>
@@ -496,10 +496,10 @@
   <dimension ref="A1:K103"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.78"/>
@@ -1066,7 +1066,7 @@
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -1086,7 +1086,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="67"/>
@@ -1130,7 +1130,7 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="lQFSRMfDnlDhurywGjcXqXjBl4WVaooXg/W0jYSgLHUX3Rb88/D74WHjGCKDdrgdHHIJvoBs4koMGgGgZOgGeA==" saltValue="q3xx4YuwomipoCR143jmTA==" spinCount="100000" sheet="true" objects="true" scenarios="true"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -1150,7 +1150,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="41.82"/>
@@ -1207,7 +1207,7 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="rnR3B9faacWpLg/dZCjGdnC4QB1ODvZ+8vO2zeJbvIf7CHGd56x4uQDZvmHOaYPCv/0BX6bhNelhSGm2z4wICw==" saltValue="o2FYOTf893qn90wx8pp9zw==" spinCount="100000" sheet="true" objects="true" scenarios="true"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>

</xml_diff>

<commit_message>
move some icons to fr-icon, fix log_edd.xlsx
</commit_message>
<xml_diff>
--- a/static/files/logements_edd.xlsx
+++ b/static/files/logements_edd.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marjo\Desktop\HD\Beta-Gouv\apilos\static\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/apilos/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762F5144-BADA-4F54-84CA-AB33F60B02C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87465EA-878A-0546-84C1-CE11EA3320B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
+    <workbookView xWindow="1240" yWindow="500" windowWidth="27560" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
   <sheets>
     <sheet name="EDD Simplifié" sheetId="1" r:id="rId1"/>
@@ -111,9 +111,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="#,##0.00\ [$€-40C]"/>
-  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -321,24 +318,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -357,6 +352,9 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,7 +452,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -753,553 +751,553 @@
   <dimension ref="A1:K102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C102" sqref="C102"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.5" customWidth="1"/>
     <col min="2" max="2" width="42.5" customWidth="1"/>
-    <col min="3" max="3" width="32" customWidth="1"/>
+    <col min="3" max="3" width="32" style="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="63" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+    <row r="2" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="A2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="13"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="13"/>
-    </row>
-    <row r="6" spans="1:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="10"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="21"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="8"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="22"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="21"/>
+    </row>
+    <row r="6" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-    </row>
-    <row r="7" spans="1:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A7" s="11"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="A7" s="10"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="13"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="13"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="13"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="13"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="13"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="13"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="13"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="13"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="13"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="9"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="13"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="9"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="13"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="9"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="13"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="9"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="11"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="13"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="9"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="11"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="13"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="9"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="11"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="13"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="9"/>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="11"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="13"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="9"/>
-      <c r="B40" s="10"/>
-      <c r="C40" s="10"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="11"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="13"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="9"/>
-      <c r="B42" s="10"/>
-      <c r="C42" s="10"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="11"/>
-      <c r="B43" s="12"/>
-      <c r="C43" s="13"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="9"/>
-      <c r="B44" s="10"/>
-      <c r="C44" s="10"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="11"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="13"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="9"/>
-      <c r="B46" s="10"/>
-      <c r="C46" s="10"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="11"/>
-      <c r="B47" s="12"/>
-      <c r="C47" s="13"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="9"/>
-      <c r="B48" s="10"/>
-      <c r="C48" s="10"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="11"/>
-      <c r="B49" s="12"/>
-      <c r="C49" s="13"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="9"/>
-      <c r="B50" s="10"/>
-      <c r="C50" s="10"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="7"/>
-      <c r="B51" s="8"/>
-      <c r="C51" s="13"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="9"/>
-      <c r="B52" s="10"/>
-      <c r="C52" s="10"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="7"/>
-      <c r="B53" s="8"/>
-      <c r="C53" s="13"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="9"/>
-      <c r="B54" s="10"/>
-      <c r="C54" s="10"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="7"/>
-      <c r="B55" s="8"/>
-      <c r="C55" s="13"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="9"/>
-      <c r="B56" s="10"/>
-      <c r="C56" s="10"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="7"/>
-      <c r="B57" s="8"/>
-      <c r="C57" s="13"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="9"/>
-      <c r="B58" s="10"/>
-      <c r="C58" s="10"/>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="7"/>
-      <c r="B59" s="8"/>
-      <c r="C59" s="13"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="9"/>
-      <c r="B60" s="10"/>
-      <c r="C60" s="10"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="7"/>
-      <c r="B61" s="8"/>
-      <c r="C61" s="13"/>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="9"/>
-      <c r="B62" s="10"/>
-      <c r="C62" s="10"/>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="7"/>
-      <c r="B63" s="8"/>
-      <c r="C63" s="13"/>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="9"/>
-      <c r="B64" s="10"/>
-      <c r="C64" s="10"/>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="7"/>
-      <c r="B65" s="8"/>
-      <c r="C65" s="13"/>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="9"/>
-      <c r="B66" s="10"/>
-      <c r="C66" s="10"/>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="7"/>
-      <c r="B67" s="8"/>
-      <c r="C67" s="13"/>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="9"/>
-      <c r="B68" s="10"/>
-      <c r="C68" s="10"/>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="7"/>
-      <c r="B69" s="8"/>
-      <c r="C69" s="13"/>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="9"/>
-      <c r="B70" s="10"/>
-      <c r="C70" s="10"/>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="7"/>
-      <c r="B71" s="8"/>
-      <c r="C71" s="13"/>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="9"/>
-      <c r="B72" s="10"/>
-      <c r="C72" s="10"/>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="7"/>
-      <c r="B73" s="8"/>
-      <c r="C73" s="13"/>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="9"/>
-      <c r="B74" s="10"/>
-      <c r="C74" s="10"/>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="7"/>
-      <c r="B75" s="8"/>
-      <c r="C75" s="13"/>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="9"/>
-      <c r="B76" s="10"/>
-      <c r="C76" s="10"/>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="7"/>
-      <c r="B77" s="8"/>
-      <c r="C77" s="13"/>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="9"/>
-      <c r="B78" s="10"/>
-      <c r="C78" s="10"/>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="7"/>
-      <c r="B79" s="8"/>
-      <c r="C79" s="13"/>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="9"/>
-      <c r="B80" s="10"/>
-      <c r="C80" s="10"/>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="7"/>
-      <c r="B81" s="8"/>
-      <c r="C81" s="13"/>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="9"/>
-      <c r="B82" s="10"/>
-      <c r="C82" s="10"/>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="7"/>
-      <c r="B83" s="8"/>
-      <c r="C83" s="13"/>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="9"/>
-      <c r="B84" s="10"/>
-      <c r="C84" s="10"/>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="7"/>
-      <c r="B85" s="8"/>
-      <c r="C85" s="13"/>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="9"/>
-      <c r="B86" s="10"/>
-      <c r="C86" s="10"/>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="7"/>
-      <c r="B87" s="8"/>
-      <c r="C87" s="13"/>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="9"/>
-      <c r="B88" s="10"/>
-      <c r="C88" s="10"/>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="7"/>
-      <c r="B89" s="8"/>
-      <c r="C89" s="13"/>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="9"/>
-      <c r="B90" s="10"/>
-      <c r="C90" s="10"/>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="7"/>
-      <c r="B91" s="8"/>
-      <c r="C91" s="13"/>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="9"/>
-      <c r="B92" s="10"/>
-      <c r="C92" s="10"/>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="7"/>
-      <c r="B93" s="8"/>
-      <c r="C93" s="13"/>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="9"/>
-      <c r="B94" s="10"/>
-      <c r="C94" s="10"/>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="7"/>
-      <c r="B95" s="8"/>
-      <c r="C95" s="13"/>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="9"/>
-      <c r="B96" s="10"/>
-      <c r="C96" s="10"/>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="7"/>
-      <c r="B97" s="8"/>
-      <c r="C97" s="13"/>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="9"/>
-      <c r="B98" s="10"/>
-      <c r="C98" s="10"/>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="7"/>
-      <c r="B99" s="8"/>
-      <c r="C99" s="13"/>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="9"/>
-      <c r="B100" s="10"/>
-      <c r="C100" s="10"/>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="7"/>
-      <c r="B101" s="8"/>
-      <c r="C101" s="13"/>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="9"/>
-      <c r="B102" s="10"/>
-      <c r="C102" s="10"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="22"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="10"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="21"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="8"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="22"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="10"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="21"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="8"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="22"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="10"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="21"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="8"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="22"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="10"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="21"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="8"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="22"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="10"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="21"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="8"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="22"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="10"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="21"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="8"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="22"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="10"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="21"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="8"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="22"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="10"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="21"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="8"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="22"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="10"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="21"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="8"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="22"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="10"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="21"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="8"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="22"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="10"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="21"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="8"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="22"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="10"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="21"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="8"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="22"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="10"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="21"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="8"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="22"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="10"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="21"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="8"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="22"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="10"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="21"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="8"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="22"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="10"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="21"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="8"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="22"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="10"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="21"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="8"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="22"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="10"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="21"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="8"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="22"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="10"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="21"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="8"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="22"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="10"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="21"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="8"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="22"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="10"/>
+      <c r="B49" s="11"/>
+      <c r="C49" s="21"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="8"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="22"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="6"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="21"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="8"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="22"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="6"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="21"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="8"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="22"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="6"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="21"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="8"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="22"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="6"/>
+      <c r="B57" s="7"/>
+      <c r="C57" s="21"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="8"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="22"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="6"/>
+      <c r="B59" s="7"/>
+      <c r="C59" s="21"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="8"/>
+      <c r="B60" s="9"/>
+      <c r="C60" s="22"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="6"/>
+      <c r="B61" s="7"/>
+      <c r="C61" s="21"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="8"/>
+      <c r="B62" s="9"/>
+      <c r="C62" s="22"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="6"/>
+      <c r="B63" s="7"/>
+      <c r="C63" s="21"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="8"/>
+      <c r="B64" s="9"/>
+      <c r="C64" s="22"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="6"/>
+      <c r="B65" s="7"/>
+      <c r="C65" s="21"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="8"/>
+      <c r="B66" s="9"/>
+      <c r="C66" s="22"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="6"/>
+      <c r="B67" s="7"/>
+      <c r="C67" s="21"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="8"/>
+      <c r="B68" s="9"/>
+      <c r="C68" s="22"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="6"/>
+      <c r="B69" s="7"/>
+      <c r="C69" s="21"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="8"/>
+      <c r="B70" s="9"/>
+      <c r="C70" s="22"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="6"/>
+      <c r="B71" s="7"/>
+      <c r="C71" s="21"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="8"/>
+      <c r="B72" s="9"/>
+      <c r="C72" s="22"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="6"/>
+      <c r="B73" s="7"/>
+      <c r="C73" s="21"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="8"/>
+      <c r="B74" s="9"/>
+      <c r="C74" s="22"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="6"/>
+      <c r="B75" s="7"/>
+      <c r="C75" s="21"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="8"/>
+      <c r="B76" s="9"/>
+      <c r="C76" s="22"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="6"/>
+      <c r="B77" s="7"/>
+      <c r="C77" s="21"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="8"/>
+      <c r="B78" s="9"/>
+      <c r="C78" s="22"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="6"/>
+      <c r="B79" s="7"/>
+      <c r="C79" s="21"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="8"/>
+      <c r="B80" s="9"/>
+      <c r="C80" s="22"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="6"/>
+      <c r="B81" s="7"/>
+      <c r="C81" s="21"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="8"/>
+      <c r="B82" s="9"/>
+      <c r="C82" s="22"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" s="6"/>
+      <c r="B83" s="7"/>
+      <c r="C83" s="21"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="8"/>
+      <c r="B84" s="9"/>
+      <c r="C84" s="22"/>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" s="6"/>
+      <c r="B85" s="7"/>
+      <c r="C85" s="21"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" s="8"/>
+      <c r="B86" s="9"/>
+      <c r="C86" s="22"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" s="6"/>
+      <c r="B87" s="7"/>
+      <c r="C87" s="21"/>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" s="8"/>
+      <c r="B88" s="9"/>
+      <c r="C88" s="22"/>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" s="6"/>
+      <c r="B89" s="7"/>
+      <c r="C89" s="21"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" s="8"/>
+      <c r="B90" s="9"/>
+      <c r="C90" s="22"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" s="6"/>
+      <c r="B91" s="7"/>
+      <c r="C91" s="21"/>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" s="8"/>
+      <c r="B92" s="9"/>
+      <c r="C92" s="22"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" s="6"/>
+      <c r="B93" s="7"/>
+      <c r="C93" s="21"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" s="8"/>
+      <c r="B94" s="9"/>
+      <c r="C94" s="22"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" s="6"/>
+      <c r="B95" s="7"/>
+      <c r="C95" s="21"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" s="8"/>
+      <c r="B96" s="9"/>
+      <c r="C96" s="22"/>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" s="6"/>
+      <c r="B97" s="7"/>
+      <c r="C97" s="21"/>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" s="8"/>
+      <c r="B98" s="9"/>
+      <c r="C98" s="22"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" s="6"/>
+      <c r="B99" s="7"/>
+      <c r="C99" s="21"/>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" s="8"/>
+      <c r="B100" s="9"/>
+      <c r="C100" s="22"/>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" s="6"/>
+      <c r="B101" s="7"/>
+      <c r="C101" s="21"/>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" s="8"/>
+      <c r="B102" s="9"/>
+      <c r="C102" s="22"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1326,43 +1324,43 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.5" customWidth="1"/>
     <col min="2" max="2" width="67" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>4</v>
       </c>
@@ -1379,58 +1377,58 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="42.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.875" customWidth="1"/>
+    <col min="3" max="3" width="41.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
move some icons to fr-icon, fix log_edd.xlsx (#285)
</commit_message>
<xml_diff>
--- a/static/files/logements_edd.xlsx
+++ b/static/files/logements_edd.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marjo\Desktop\HD\Beta-Gouv\apilos\static\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/apilos/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762F5144-BADA-4F54-84CA-AB33F60B02C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87465EA-878A-0546-84C1-CE11EA3320B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
+    <workbookView xWindow="1240" yWindow="500" windowWidth="27560" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
   <sheets>
     <sheet name="EDD Simplifié" sheetId="1" r:id="rId1"/>
@@ -111,9 +111,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="#,##0.00\ [$€-40C]"/>
-  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -321,24 +318,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -357,6 +352,9 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,7 +452,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -753,553 +751,553 @@
   <dimension ref="A1:K102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C102" sqref="C102"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.5" customWidth="1"/>
     <col min="2" max="2" width="42.5" customWidth="1"/>
-    <col min="3" max="3" width="32" customWidth="1"/>
+    <col min="3" max="3" width="32" style="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="63" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+    <row r="2" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="A2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="13"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="13"/>
-    </row>
-    <row r="6" spans="1:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="10"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="21"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="8"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="22"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="21"/>
+    </row>
+    <row r="6" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-    </row>
-    <row r="7" spans="1:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A7" s="11"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="A7" s="10"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="13"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="13"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="13"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="13"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="13"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="13"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="13"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="13"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="13"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="9"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="13"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="9"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="13"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="9"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="13"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="9"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="11"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="13"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="9"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="11"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="13"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="9"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="11"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="13"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="9"/>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="11"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="13"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="9"/>
-      <c r="B40" s="10"/>
-      <c r="C40" s="10"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="11"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="13"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="9"/>
-      <c r="B42" s="10"/>
-      <c r="C42" s="10"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="11"/>
-      <c r="B43" s="12"/>
-      <c r="C43" s="13"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="9"/>
-      <c r="B44" s="10"/>
-      <c r="C44" s="10"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="11"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="13"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="9"/>
-      <c r="B46" s="10"/>
-      <c r="C46" s="10"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="11"/>
-      <c r="B47" s="12"/>
-      <c r="C47" s="13"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="9"/>
-      <c r="B48" s="10"/>
-      <c r="C48" s="10"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="11"/>
-      <c r="B49" s="12"/>
-      <c r="C49" s="13"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="9"/>
-      <c r="B50" s="10"/>
-      <c r="C50" s="10"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="7"/>
-      <c r="B51" s="8"/>
-      <c r="C51" s="13"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="9"/>
-      <c r="B52" s="10"/>
-      <c r="C52" s="10"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="7"/>
-      <c r="B53" s="8"/>
-      <c r="C53" s="13"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="9"/>
-      <c r="B54" s="10"/>
-      <c r="C54" s="10"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="7"/>
-      <c r="B55" s="8"/>
-      <c r="C55" s="13"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="9"/>
-      <c r="B56" s="10"/>
-      <c r="C56" s="10"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="7"/>
-      <c r="B57" s="8"/>
-      <c r="C57" s="13"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="9"/>
-      <c r="B58" s="10"/>
-      <c r="C58" s="10"/>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="7"/>
-      <c r="B59" s="8"/>
-      <c r="C59" s="13"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="9"/>
-      <c r="B60" s="10"/>
-      <c r="C60" s="10"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="7"/>
-      <c r="B61" s="8"/>
-      <c r="C61" s="13"/>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="9"/>
-      <c r="B62" s="10"/>
-      <c r="C62" s="10"/>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="7"/>
-      <c r="B63" s="8"/>
-      <c r="C63" s="13"/>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="9"/>
-      <c r="B64" s="10"/>
-      <c r="C64" s="10"/>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="7"/>
-      <c r="B65" s="8"/>
-      <c r="C65" s="13"/>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="9"/>
-      <c r="B66" s="10"/>
-      <c r="C66" s="10"/>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="7"/>
-      <c r="B67" s="8"/>
-      <c r="C67" s="13"/>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="9"/>
-      <c r="B68" s="10"/>
-      <c r="C68" s="10"/>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="7"/>
-      <c r="B69" s="8"/>
-      <c r="C69" s="13"/>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="9"/>
-      <c r="B70" s="10"/>
-      <c r="C70" s="10"/>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="7"/>
-      <c r="B71" s="8"/>
-      <c r="C71" s="13"/>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="9"/>
-      <c r="B72" s="10"/>
-      <c r="C72" s="10"/>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="7"/>
-      <c r="B73" s="8"/>
-      <c r="C73" s="13"/>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="9"/>
-      <c r="B74" s="10"/>
-      <c r="C74" s="10"/>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="7"/>
-      <c r="B75" s="8"/>
-      <c r="C75" s="13"/>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="9"/>
-      <c r="B76" s="10"/>
-      <c r="C76" s="10"/>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="7"/>
-      <c r="B77" s="8"/>
-      <c r="C77" s="13"/>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="9"/>
-      <c r="B78" s="10"/>
-      <c r="C78" s="10"/>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="7"/>
-      <c r="B79" s="8"/>
-      <c r="C79" s="13"/>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="9"/>
-      <c r="B80" s="10"/>
-      <c r="C80" s="10"/>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="7"/>
-      <c r="B81" s="8"/>
-      <c r="C81" s="13"/>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="9"/>
-      <c r="B82" s="10"/>
-      <c r="C82" s="10"/>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="7"/>
-      <c r="B83" s="8"/>
-      <c r="C83" s="13"/>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="9"/>
-      <c r="B84" s="10"/>
-      <c r="C84" s="10"/>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="7"/>
-      <c r="B85" s="8"/>
-      <c r="C85" s="13"/>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="9"/>
-      <c r="B86" s="10"/>
-      <c r="C86" s="10"/>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="7"/>
-      <c r="B87" s="8"/>
-      <c r="C87" s="13"/>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="9"/>
-      <c r="B88" s="10"/>
-      <c r="C88" s="10"/>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="7"/>
-      <c r="B89" s="8"/>
-      <c r="C89" s="13"/>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="9"/>
-      <c r="B90" s="10"/>
-      <c r="C90" s="10"/>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="7"/>
-      <c r="B91" s="8"/>
-      <c r="C91" s="13"/>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="9"/>
-      <c r="B92" s="10"/>
-      <c r="C92" s="10"/>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="7"/>
-      <c r="B93" s="8"/>
-      <c r="C93" s="13"/>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="9"/>
-      <c r="B94" s="10"/>
-      <c r="C94" s="10"/>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="7"/>
-      <c r="B95" s="8"/>
-      <c r="C95" s="13"/>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="9"/>
-      <c r="B96" s="10"/>
-      <c r="C96" s="10"/>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="7"/>
-      <c r="B97" s="8"/>
-      <c r="C97" s="13"/>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="9"/>
-      <c r="B98" s="10"/>
-      <c r="C98" s="10"/>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="7"/>
-      <c r="B99" s="8"/>
-      <c r="C99" s="13"/>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="9"/>
-      <c r="B100" s="10"/>
-      <c r="C100" s="10"/>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="7"/>
-      <c r="B101" s="8"/>
-      <c r="C101" s="13"/>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="9"/>
-      <c r="B102" s="10"/>
-      <c r="C102" s="10"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="22"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="10"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="21"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="8"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="22"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="10"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="21"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="8"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="22"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="10"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="21"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="8"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="22"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="10"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="21"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="8"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="22"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="10"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="21"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="8"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="22"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="10"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="21"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="8"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="22"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="10"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="21"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="8"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="22"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="10"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="21"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="8"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="22"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="10"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="21"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="8"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="22"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="10"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="21"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="8"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="22"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="10"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="21"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="8"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="22"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="10"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="21"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="8"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="22"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="10"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="21"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="8"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="22"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="10"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="21"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="8"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="22"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="10"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="21"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="8"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="22"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="10"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="21"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="8"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="22"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="10"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="21"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="8"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="22"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="10"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="21"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="8"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="22"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="10"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="21"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="8"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="22"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="10"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="21"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="8"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="22"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="10"/>
+      <c r="B49" s="11"/>
+      <c r="C49" s="21"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="8"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="22"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="6"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="21"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="8"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="22"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="6"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="21"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="8"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="22"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="6"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="21"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="8"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="22"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="6"/>
+      <c r="B57" s="7"/>
+      <c r="C57" s="21"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="8"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="22"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="6"/>
+      <c r="B59" s="7"/>
+      <c r="C59" s="21"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="8"/>
+      <c r="B60" s="9"/>
+      <c r="C60" s="22"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="6"/>
+      <c r="B61" s="7"/>
+      <c r="C61" s="21"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="8"/>
+      <c r="B62" s="9"/>
+      <c r="C62" s="22"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="6"/>
+      <c r="B63" s="7"/>
+      <c r="C63" s="21"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="8"/>
+      <c r="B64" s="9"/>
+      <c r="C64" s="22"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="6"/>
+      <c r="B65" s="7"/>
+      <c r="C65" s="21"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="8"/>
+      <c r="B66" s="9"/>
+      <c r="C66" s="22"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="6"/>
+      <c r="B67" s="7"/>
+      <c r="C67" s="21"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="8"/>
+      <c r="B68" s="9"/>
+      <c r="C68" s="22"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="6"/>
+      <c r="B69" s="7"/>
+      <c r="C69" s="21"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="8"/>
+      <c r="B70" s="9"/>
+      <c r="C70" s="22"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="6"/>
+      <c r="B71" s="7"/>
+      <c r="C71" s="21"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="8"/>
+      <c r="B72" s="9"/>
+      <c r="C72" s="22"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="6"/>
+      <c r="B73" s="7"/>
+      <c r="C73" s="21"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="8"/>
+      <c r="B74" s="9"/>
+      <c r="C74" s="22"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="6"/>
+      <c r="B75" s="7"/>
+      <c r="C75" s="21"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="8"/>
+      <c r="B76" s="9"/>
+      <c r="C76" s="22"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="6"/>
+      <c r="B77" s="7"/>
+      <c r="C77" s="21"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="8"/>
+      <c r="B78" s="9"/>
+      <c r="C78" s="22"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="6"/>
+      <c r="B79" s="7"/>
+      <c r="C79" s="21"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="8"/>
+      <c r="B80" s="9"/>
+      <c r="C80" s="22"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="6"/>
+      <c r="B81" s="7"/>
+      <c r="C81" s="21"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="8"/>
+      <c r="B82" s="9"/>
+      <c r="C82" s="22"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" s="6"/>
+      <c r="B83" s="7"/>
+      <c r="C83" s="21"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="8"/>
+      <c r="B84" s="9"/>
+      <c r="C84" s="22"/>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" s="6"/>
+      <c r="B85" s="7"/>
+      <c r="C85" s="21"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" s="8"/>
+      <c r="B86" s="9"/>
+      <c r="C86" s="22"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" s="6"/>
+      <c r="B87" s="7"/>
+      <c r="C87" s="21"/>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" s="8"/>
+      <c r="B88" s="9"/>
+      <c r="C88" s="22"/>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" s="6"/>
+      <c r="B89" s="7"/>
+      <c r="C89" s="21"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" s="8"/>
+      <c r="B90" s="9"/>
+      <c r="C90" s="22"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" s="6"/>
+      <c r="B91" s="7"/>
+      <c r="C91" s="21"/>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" s="8"/>
+      <c r="B92" s="9"/>
+      <c r="C92" s="22"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" s="6"/>
+      <c r="B93" s="7"/>
+      <c r="C93" s="21"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" s="8"/>
+      <c r="B94" s="9"/>
+      <c r="C94" s="22"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" s="6"/>
+      <c r="B95" s="7"/>
+      <c r="C95" s="21"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" s="8"/>
+      <c r="B96" s="9"/>
+      <c r="C96" s="22"/>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" s="6"/>
+      <c r="B97" s="7"/>
+      <c r="C97" s="21"/>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" s="8"/>
+      <c r="B98" s="9"/>
+      <c r="C98" s="22"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" s="6"/>
+      <c r="B99" s="7"/>
+      <c r="C99" s="21"/>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" s="8"/>
+      <c r="B100" s="9"/>
+      <c r="C100" s="22"/>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" s="6"/>
+      <c r="B101" s="7"/>
+      <c r="C101" s="21"/>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" s="8"/>
+      <c r="B102" s="9"/>
+      <c r="C102" s="22"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1326,43 +1324,43 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.5" customWidth="1"/>
     <col min="2" max="2" width="67" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>4</v>
       </c>
@@ -1379,58 +1377,58 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="42.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.875" customWidth="1"/>
+    <col min="3" max="3" width="41.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
s622: remove PLAI_ADP from available options to create EDD or new conventions
</commit_message>
<xml_diff>
--- a/static/files/logements_edd.xlsx
+++ b/static/files/logements_edd.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/apilos/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87465EA-878A-0546-84C1-CE11EA3320B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2707DDD9-7FCB-FD47-86AA-0F39F1CB4F79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1240" yWindow="500" windowWidth="27560" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Ici quelques explications</t>
   </si>
@@ -81,9 +81,6 @@
   </si>
   <si>
     <t>PLAI</t>
-  </si>
-  <si>
-    <t>PLAI_ADP</t>
   </si>
   <si>
     <t>PLS</t>
@@ -318,7 +315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -352,9 +349,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -750,15 +745,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08021C90-1ACF-2A4C-A1B0-58A48A8F7007}">
   <dimension ref="A1:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.5" customWidth="1"/>
     <col min="2" max="2" width="42.5" customWidth="1"/>
-    <col min="3" max="3" width="32" style="23" customWidth="1"/>
+    <col min="3" max="3" width="32" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
@@ -769,18 +762,18 @@
         <v>11</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="19" t="s">
-        <v>20</v>
-      </c>
       <c r="C2" s="20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -791,7 +784,7 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="9"/>
-      <c r="C4" s="22"/>
+      <c r="C4" s="9"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="10"/>
@@ -801,7 +794,7 @@
     <row r="6" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="A6" s="8"/>
       <c r="B6" s="9"/>
-      <c r="C6" s="22"/>
+      <c r="C6" s="9"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -827,7 +820,7 @@
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="8"/>
       <c r="B8" s="9"/>
-      <c r="C8" s="22"/>
+      <c r="C8" s="9"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="10"/>
@@ -837,7 +830,7 @@
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
       <c r="B10" s="9"/>
-      <c r="C10" s="22"/>
+      <c r="C10" s="9"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="10"/>
@@ -847,7 +840,7 @@
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
-      <c r="C12" s="22"/>
+      <c r="C12" s="9"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="10"/>
@@ -857,7 +850,7 @@
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
       <c r="B14" s="9"/>
-      <c r="C14" s="22"/>
+      <c r="C14" s="9"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="10"/>
@@ -867,7 +860,7 @@
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
       <c r="B16" s="9"/>
-      <c r="C16" s="22"/>
+      <c r="C16" s="9"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="10"/>
@@ -877,7 +870,7 @@
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="8"/>
       <c r="B18" s="9"/>
-      <c r="C18" s="22"/>
+      <c r="C18" s="9"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="10"/>
@@ -887,7 +880,7 @@
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="8"/>
       <c r="B20" s="9"/>
-      <c r="C20" s="22"/>
+      <c r="C20" s="9"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="10"/>
@@ -897,7 +890,7 @@
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="8"/>
       <c r="B22" s="9"/>
-      <c r="C22" s="22"/>
+      <c r="C22" s="9"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="10"/>
@@ -907,7 +900,7 @@
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="8"/>
       <c r="B24" s="9"/>
-      <c r="C24" s="22"/>
+      <c r="C24" s="9"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="10"/>
@@ -917,7 +910,7 @@
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="8"/>
       <c r="B26" s="9"/>
-      <c r="C26" s="22"/>
+      <c r="C26" s="9"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="10"/>
@@ -927,7 +920,7 @@
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="8"/>
       <c r="B28" s="9"/>
-      <c r="C28" s="22"/>
+      <c r="C28" s="9"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="10"/>
@@ -937,7 +930,7 @@
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="8"/>
       <c r="B30" s="9"/>
-      <c r="C30" s="22"/>
+      <c r="C30" s="9"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="10"/>
@@ -947,7 +940,7 @@
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="8"/>
       <c r="B32" s="9"/>
-      <c r="C32" s="22"/>
+      <c r="C32" s="9"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="10"/>
@@ -957,7 +950,7 @@
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="8"/>
       <c r="B34" s="9"/>
-      <c r="C34" s="22"/>
+      <c r="C34" s="9"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="10"/>
@@ -967,7 +960,7 @@
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="8"/>
       <c r="B36" s="9"/>
-      <c r="C36" s="22"/>
+      <c r="C36" s="9"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="10"/>
@@ -977,7 +970,7 @@
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="8"/>
       <c r="B38" s="9"/>
-      <c r="C38" s="22"/>
+      <c r="C38" s="9"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="10"/>
@@ -987,7 +980,7 @@
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="8"/>
       <c r="B40" s="9"/>
-      <c r="C40" s="22"/>
+      <c r="C40" s="9"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="10"/>
@@ -997,7 +990,7 @@
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="8"/>
       <c r="B42" s="9"/>
-      <c r="C42" s="22"/>
+      <c r="C42" s="9"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="10"/>
@@ -1007,7 +1000,7 @@
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="8"/>
       <c r="B44" s="9"/>
-      <c r="C44" s="22"/>
+      <c r="C44" s="9"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="10"/>
@@ -1017,7 +1010,7 @@
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="8"/>
       <c r="B46" s="9"/>
-      <c r="C46" s="22"/>
+      <c r="C46" s="9"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="10"/>
@@ -1027,7 +1020,7 @@
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="8"/>
       <c r="B48" s="9"/>
-      <c r="C48" s="22"/>
+      <c r="C48" s="9"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="10"/>
@@ -1037,7 +1030,7 @@
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="8"/>
       <c r="B50" s="9"/>
-      <c r="C50" s="22"/>
+      <c r="C50" s="9"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="6"/>
@@ -1047,7 +1040,7 @@
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="8"/>
       <c r="B52" s="9"/>
-      <c r="C52" s="22"/>
+      <c r="C52" s="9"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="6"/>
@@ -1057,7 +1050,7 @@
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="8"/>
       <c r="B54" s="9"/>
-      <c r="C54" s="22"/>
+      <c r="C54" s="9"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="6"/>
@@ -1067,7 +1060,7 @@
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="8"/>
       <c r="B56" s="9"/>
-      <c r="C56" s="22"/>
+      <c r="C56" s="9"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="6"/>
@@ -1077,7 +1070,7 @@
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="8"/>
       <c r="B58" s="9"/>
-      <c r="C58" s="22"/>
+      <c r="C58" s="9"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="6"/>
@@ -1087,7 +1080,7 @@
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="8"/>
       <c r="B60" s="9"/>
-      <c r="C60" s="22"/>
+      <c r="C60" s="9"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="6"/>
@@ -1097,7 +1090,7 @@
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="8"/>
       <c r="B62" s="9"/>
-      <c r="C62" s="22"/>
+      <c r="C62" s="9"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="6"/>
@@ -1107,7 +1100,7 @@
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="8"/>
       <c r="B64" s="9"/>
-      <c r="C64" s="22"/>
+      <c r="C64" s="9"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="6"/>
@@ -1117,7 +1110,7 @@
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="8"/>
       <c r="B66" s="9"/>
-      <c r="C66" s="22"/>
+      <c r="C66" s="9"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="6"/>
@@ -1127,7 +1120,7 @@
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="8"/>
       <c r="B68" s="9"/>
-      <c r="C68" s="22"/>
+      <c r="C68" s="9"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="6"/>
@@ -1137,7 +1130,7 @@
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="8"/>
       <c r="B70" s="9"/>
-      <c r="C70" s="22"/>
+      <c r="C70" s="9"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="6"/>
@@ -1147,7 +1140,7 @@
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="8"/>
       <c r="B72" s="9"/>
-      <c r="C72" s="22"/>
+      <c r="C72" s="9"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="6"/>
@@ -1157,7 +1150,7 @@
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="8"/>
       <c r="B74" s="9"/>
-      <c r="C74" s="22"/>
+      <c r="C74" s="9"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="6"/>
@@ -1167,7 +1160,7 @@
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="8"/>
       <c r="B76" s="9"/>
-      <c r="C76" s="22"/>
+      <c r="C76" s="9"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="6"/>
@@ -1177,7 +1170,7 @@
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="8"/>
       <c r="B78" s="9"/>
-      <c r="C78" s="22"/>
+      <c r="C78" s="9"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="6"/>
@@ -1187,7 +1180,7 @@
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="8"/>
       <c r="B80" s="9"/>
-      <c r="C80" s="22"/>
+      <c r="C80" s="9"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="6"/>
@@ -1197,7 +1190,7 @@
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="8"/>
       <c r="B82" s="9"/>
-      <c r="C82" s="22"/>
+      <c r="C82" s="9"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="6"/>
@@ -1207,7 +1200,7 @@
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="8"/>
       <c r="B84" s="9"/>
-      <c r="C84" s="22"/>
+      <c r="C84" s="9"/>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="6"/>
@@ -1217,7 +1210,7 @@
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="8"/>
       <c r="B86" s="9"/>
-      <c r="C86" s="22"/>
+      <c r="C86" s="9"/>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="6"/>
@@ -1227,7 +1220,7 @@
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="8"/>
       <c r="B88" s="9"/>
-      <c r="C88" s="22"/>
+      <c r="C88" s="9"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="6"/>
@@ -1237,7 +1230,7 @@
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="8"/>
       <c r="B90" s="9"/>
-      <c r="C90" s="22"/>
+      <c r="C90" s="9"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="6"/>
@@ -1247,7 +1240,7 @@
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="8"/>
       <c r="B92" s="9"/>
-      <c r="C92" s="22"/>
+      <c r="C92" s="9"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="6"/>
@@ -1257,7 +1250,7 @@
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="8"/>
       <c r="B94" s="9"/>
-      <c r="C94" s="22"/>
+      <c r="C94" s="9"/>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="6"/>
@@ -1267,7 +1260,7 @@
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="8"/>
       <c r="B96" s="9"/>
-      <c r="C96" s="22"/>
+      <c r="C96" s="9"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="6"/>
@@ -1277,7 +1270,7 @@
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="8"/>
       <c r="B98" s="9"/>
-      <c r="C98" s="22"/>
+      <c r="C98" s="9"/>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="6"/>
@@ -1287,7 +1280,7 @@
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="8"/>
       <c r="B100" s="9"/>
-      <c r="C100" s="22"/>
+      <c r="C100" s="9"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="6"/>
@@ -1297,7 +1290,7 @@
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="8"/>
       <c r="B102" s="9"/>
-      <c r="C102" s="22"/>
+      <c r="C102" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1308,7 +1301,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{175F71C0-CCE8-034C-8D7C-791DB0178004}">
           <x14:formula1>
-            <xm:f>Data!$C$2:$C$5</xm:f>
+            <xm:f>Data!$C$2:$C$4</xm:f>
           </x14:formula1>
           <xm:sqref>A3:A102</xm:sqref>
         </x14:dataValidation>
@@ -1342,7 +1335,7 @@
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.2">
@@ -1357,7 +1350,7 @@
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.2">
@@ -1419,9 +1412,6 @@
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="14" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -1432,7 +1422,7 @@
       <c r="A7" s="4"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="rnR3B9faacWpLg/dZCjGdnC4QB1ODvZ+8vO2zeJbvIf7CHGd56x4uQDZvmHOaYPCv/0BX6bhNelhSGm2z4wICw==" saltValue="o2FYOTf893qn90wx8pp9zw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="wnNF8dq4EQlAY3bw6Oejp7mW6UNCmjFIQvL86ndQn11xSnojYGhb8UEkkCGgZQaueviKI+2rXi9ZBo9BcThcEw==" saltValue="j9JeVYPBr1R2l4bt0sisbA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
s622: remove PLAI_ADP from available options to create EDD or new conventions (#395)
</commit_message>
<xml_diff>
--- a/static/files/logements_edd.xlsx
+++ b/static/files/logements_edd.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/apilos/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87465EA-878A-0546-84C1-CE11EA3320B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2707DDD9-7FCB-FD47-86AA-0F39F1CB4F79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1240" yWindow="500" windowWidth="27560" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Ici quelques explications</t>
   </si>
@@ -81,9 +81,6 @@
   </si>
   <si>
     <t>PLAI</t>
-  </si>
-  <si>
-    <t>PLAI_ADP</t>
   </si>
   <si>
     <t>PLS</t>
@@ -318,7 +315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -352,9 +349,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -750,15 +745,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08021C90-1ACF-2A4C-A1B0-58A48A8F7007}">
   <dimension ref="A1:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.5" customWidth="1"/>
     <col min="2" max="2" width="42.5" customWidth="1"/>
-    <col min="3" max="3" width="32" style="23" customWidth="1"/>
+    <col min="3" max="3" width="32" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
@@ -769,18 +762,18 @@
         <v>11</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="19" t="s">
-        <v>20</v>
-      </c>
       <c r="C2" s="20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -791,7 +784,7 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="9"/>
-      <c r="C4" s="22"/>
+      <c r="C4" s="9"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="10"/>
@@ -801,7 +794,7 @@
     <row r="6" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="A6" s="8"/>
       <c r="B6" s="9"/>
-      <c r="C6" s="22"/>
+      <c r="C6" s="9"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -827,7 +820,7 @@
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="8"/>
       <c r="B8" s="9"/>
-      <c r="C8" s="22"/>
+      <c r="C8" s="9"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="10"/>
@@ -837,7 +830,7 @@
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
       <c r="B10" s="9"/>
-      <c r="C10" s="22"/>
+      <c r="C10" s="9"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="10"/>
@@ -847,7 +840,7 @@
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
-      <c r="C12" s="22"/>
+      <c r="C12" s="9"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="10"/>
@@ -857,7 +850,7 @@
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
       <c r="B14" s="9"/>
-      <c r="C14" s="22"/>
+      <c r="C14" s="9"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="10"/>
@@ -867,7 +860,7 @@
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
       <c r="B16" s="9"/>
-      <c r="C16" s="22"/>
+      <c r="C16" s="9"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="10"/>
@@ -877,7 +870,7 @@
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="8"/>
       <c r="B18" s="9"/>
-      <c r="C18" s="22"/>
+      <c r="C18" s="9"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="10"/>
@@ -887,7 +880,7 @@
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="8"/>
       <c r="B20" s="9"/>
-      <c r="C20" s="22"/>
+      <c r="C20" s="9"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="10"/>
@@ -897,7 +890,7 @@
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="8"/>
       <c r="B22" s="9"/>
-      <c r="C22" s="22"/>
+      <c r="C22" s="9"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="10"/>
@@ -907,7 +900,7 @@
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="8"/>
       <c r="B24" s="9"/>
-      <c r="C24" s="22"/>
+      <c r="C24" s="9"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="10"/>
@@ -917,7 +910,7 @@
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="8"/>
       <c r="B26" s="9"/>
-      <c r="C26" s="22"/>
+      <c r="C26" s="9"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="10"/>
@@ -927,7 +920,7 @@
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="8"/>
       <c r="B28" s="9"/>
-      <c r="C28" s="22"/>
+      <c r="C28" s="9"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="10"/>
@@ -937,7 +930,7 @@
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="8"/>
       <c r="B30" s="9"/>
-      <c r="C30" s="22"/>
+      <c r="C30" s="9"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="10"/>
@@ -947,7 +940,7 @@
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="8"/>
       <c r="B32" s="9"/>
-      <c r="C32" s="22"/>
+      <c r="C32" s="9"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="10"/>
@@ -957,7 +950,7 @@
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="8"/>
       <c r="B34" s="9"/>
-      <c r="C34" s="22"/>
+      <c r="C34" s="9"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="10"/>
@@ -967,7 +960,7 @@
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="8"/>
       <c r="B36" s="9"/>
-      <c r="C36" s="22"/>
+      <c r="C36" s="9"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="10"/>
@@ -977,7 +970,7 @@
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="8"/>
       <c r="B38" s="9"/>
-      <c r="C38" s="22"/>
+      <c r="C38" s="9"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="10"/>
@@ -987,7 +980,7 @@
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="8"/>
       <c r="B40" s="9"/>
-      <c r="C40" s="22"/>
+      <c r="C40" s="9"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="10"/>
@@ -997,7 +990,7 @@
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="8"/>
       <c r="B42" s="9"/>
-      <c r="C42" s="22"/>
+      <c r="C42" s="9"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="10"/>
@@ -1007,7 +1000,7 @@
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="8"/>
       <c r="B44" s="9"/>
-      <c r="C44" s="22"/>
+      <c r="C44" s="9"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="10"/>
@@ -1017,7 +1010,7 @@
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="8"/>
       <c r="B46" s="9"/>
-      <c r="C46" s="22"/>
+      <c r="C46" s="9"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="10"/>
@@ -1027,7 +1020,7 @@
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="8"/>
       <c r="B48" s="9"/>
-      <c r="C48" s="22"/>
+      <c r="C48" s="9"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="10"/>
@@ -1037,7 +1030,7 @@
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="8"/>
       <c r="B50" s="9"/>
-      <c r="C50" s="22"/>
+      <c r="C50" s="9"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="6"/>
@@ -1047,7 +1040,7 @@
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="8"/>
       <c r="B52" s="9"/>
-      <c r="C52" s="22"/>
+      <c r="C52" s="9"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="6"/>
@@ -1057,7 +1050,7 @@
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="8"/>
       <c r="B54" s="9"/>
-      <c r="C54" s="22"/>
+      <c r="C54" s="9"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="6"/>
@@ -1067,7 +1060,7 @@
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="8"/>
       <c r="B56" s="9"/>
-      <c r="C56" s="22"/>
+      <c r="C56" s="9"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="6"/>
@@ -1077,7 +1070,7 @@
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="8"/>
       <c r="B58" s="9"/>
-      <c r="C58" s="22"/>
+      <c r="C58" s="9"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="6"/>
@@ -1087,7 +1080,7 @@
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="8"/>
       <c r="B60" s="9"/>
-      <c r="C60" s="22"/>
+      <c r="C60" s="9"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="6"/>
@@ -1097,7 +1090,7 @@
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="8"/>
       <c r="B62" s="9"/>
-      <c r="C62" s="22"/>
+      <c r="C62" s="9"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="6"/>
@@ -1107,7 +1100,7 @@
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="8"/>
       <c r="B64" s="9"/>
-      <c r="C64" s="22"/>
+      <c r="C64" s="9"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="6"/>
@@ -1117,7 +1110,7 @@
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="8"/>
       <c r="B66" s="9"/>
-      <c r="C66" s="22"/>
+      <c r="C66" s="9"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="6"/>
@@ -1127,7 +1120,7 @@
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="8"/>
       <c r="B68" s="9"/>
-      <c r="C68" s="22"/>
+      <c r="C68" s="9"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="6"/>
@@ -1137,7 +1130,7 @@
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="8"/>
       <c r="B70" s="9"/>
-      <c r="C70" s="22"/>
+      <c r="C70" s="9"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="6"/>
@@ -1147,7 +1140,7 @@
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="8"/>
       <c r="B72" s="9"/>
-      <c r="C72" s="22"/>
+      <c r="C72" s="9"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="6"/>
@@ -1157,7 +1150,7 @@
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="8"/>
       <c r="B74" s="9"/>
-      <c r="C74" s="22"/>
+      <c r="C74" s="9"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="6"/>
@@ -1167,7 +1160,7 @@
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="8"/>
       <c r="B76" s="9"/>
-      <c r="C76" s="22"/>
+      <c r="C76" s="9"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="6"/>
@@ -1177,7 +1170,7 @@
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="8"/>
       <c r="B78" s="9"/>
-      <c r="C78" s="22"/>
+      <c r="C78" s="9"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="6"/>
@@ -1187,7 +1180,7 @@
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="8"/>
       <c r="B80" s="9"/>
-      <c r="C80" s="22"/>
+      <c r="C80" s="9"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="6"/>
@@ -1197,7 +1190,7 @@
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="8"/>
       <c r="B82" s="9"/>
-      <c r="C82" s="22"/>
+      <c r="C82" s="9"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="6"/>
@@ -1207,7 +1200,7 @@
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="8"/>
       <c r="B84" s="9"/>
-      <c r="C84" s="22"/>
+      <c r="C84" s="9"/>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="6"/>
@@ -1217,7 +1210,7 @@
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="8"/>
       <c r="B86" s="9"/>
-      <c r="C86" s="22"/>
+      <c r="C86" s="9"/>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="6"/>
@@ -1227,7 +1220,7 @@
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="8"/>
       <c r="B88" s="9"/>
-      <c r="C88" s="22"/>
+      <c r="C88" s="9"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="6"/>
@@ -1237,7 +1230,7 @@
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="8"/>
       <c r="B90" s="9"/>
-      <c r="C90" s="22"/>
+      <c r="C90" s="9"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="6"/>
@@ -1247,7 +1240,7 @@
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="8"/>
       <c r="B92" s="9"/>
-      <c r="C92" s="22"/>
+      <c r="C92" s="9"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="6"/>
@@ -1257,7 +1250,7 @@
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="8"/>
       <c r="B94" s="9"/>
-      <c r="C94" s="22"/>
+      <c r="C94" s="9"/>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="6"/>
@@ -1267,7 +1260,7 @@
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="8"/>
       <c r="B96" s="9"/>
-      <c r="C96" s="22"/>
+      <c r="C96" s="9"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="6"/>
@@ -1277,7 +1270,7 @@
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="8"/>
       <c r="B98" s="9"/>
-      <c r="C98" s="22"/>
+      <c r="C98" s="9"/>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="6"/>
@@ -1287,7 +1280,7 @@
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="8"/>
       <c r="B100" s="9"/>
-      <c r="C100" s="22"/>
+      <c r="C100" s="9"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="6"/>
@@ -1297,7 +1290,7 @@
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="8"/>
       <c r="B102" s="9"/>
-      <c r="C102" s="22"/>
+      <c r="C102" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1308,7 +1301,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{175F71C0-CCE8-034C-8D7C-791DB0178004}">
           <x14:formula1>
-            <xm:f>Data!$C$2:$C$5</xm:f>
+            <xm:f>Data!$C$2:$C$4</xm:f>
           </x14:formula1>
           <xm:sqref>A3:A102</xm:sqref>
         </x14:dataValidation>
@@ -1342,7 +1335,7 @@
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.2">
@@ -1357,7 +1350,7 @@
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.2">
@@ -1419,9 +1412,6 @@
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="14" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -1432,7 +1422,7 @@
       <c r="A7" s="4"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="rnR3B9faacWpLg/dZCjGdnC4QB1ODvZ+8vO2zeJbvIf7CHGd56x4uQDZvmHOaYPCv/0BX6bhNelhSGm2z4wICw==" saltValue="o2FYOTf893qn90wx8pp9zw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="wnNF8dq4EQlAY3bw6Oejp7mW6UNCmjFIQvL86ndQn11xSnojYGhb8UEkkCGgZQaueviKI+2rXi9ZBo9BcThcEw==" saltValue="j9JeVYPBr1R2l4bt0sisbA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Revert "s652_Json staging (#399)"
This reverts commit 3641673445830232613622ae0f47b045bdbd2e14.
</commit_message>
<xml_diff>
--- a/static/files/logements_edd.xlsx
+++ b/static/files/logements_edd.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/apilos/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87465EA-878A-0546-84C1-CE11EA3320B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2707DDD9-7FCB-FD47-86AA-0F39F1CB4F79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1240" yWindow="500" windowWidth="27560" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Ici quelques explications</t>
   </si>
@@ -81,9 +81,6 @@
   </si>
   <si>
     <t>PLAI</t>
-  </si>
-  <si>
-    <t>PLAI_ADP</t>
   </si>
   <si>
     <t>PLS</t>
@@ -318,7 +315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -352,9 +349,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -750,15 +745,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08021C90-1ACF-2A4C-A1B0-58A48A8F7007}">
   <dimension ref="A1:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.5" customWidth="1"/>
     <col min="2" max="2" width="42.5" customWidth="1"/>
-    <col min="3" max="3" width="32" style="23" customWidth="1"/>
+    <col min="3" max="3" width="32" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
@@ -769,18 +762,18 @@
         <v>11</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="19" t="s">
-        <v>20</v>
-      </c>
       <c r="C2" s="20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -791,7 +784,7 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="9"/>
-      <c r="C4" s="22"/>
+      <c r="C4" s="9"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="10"/>
@@ -801,7 +794,7 @@
     <row r="6" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="A6" s="8"/>
       <c r="B6" s="9"/>
-      <c r="C6" s="22"/>
+      <c r="C6" s="9"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -827,7 +820,7 @@
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="8"/>
       <c r="B8" s="9"/>
-      <c r="C8" s="22"/>
+      <c r="C8" s="9"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="10"/>
@@ -837,7 +830,7 @@
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
       <c r="B10" s="9"/>
-      <c r="C10" s="22"/>
+      <c r="C10" s="9"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="10"/>
@@ -847,7 +840,7 @@
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
-      <c r="C12" s="22"/>
+      <c r="C12" s="9"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="10"/>
@@ -857,7 +850,7 @@
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
       <c r="B14" s="9"/>
-      <c r="C14" s="22"/>
+      <c r="C14" s="9"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="10"/>
@@ -867,7 +860,7 @@
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
       <c r="B16" s="9"/>
-      <c r="C16" s="22"/>
+      <c r="C16" s="9"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="10"/>
@@ -877,7 +870,7 @@
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="8"/>
       <c r="B18" s="9"/>
-      <c r="C18" s="22"/>
+      <c r="C18" s="9"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="10"/>
@@ -887,7 +880,7 @@
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="8"/>
       <c r="B20" s="9"/>
-      <c r="C20" s="22"/>
+      <c r="C20" s="9"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="10"/>
@@ -897,7 +890,7 @@
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="8"/>
       <c r="B22" s="9"/>
-      <c r="C22" s="22"/>
+      <c r="C22" s="9"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="10"/>
@@ -907,7 +900,7 @@
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="8"/>
       <c r="B24" s="9"/>
-      <c r="C24" s="22"/>
+      <c r="C24" s="9"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="10"/>
@@ -917,7 +910,7 @@
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="8"/>
       <c r="B26" s="9"/>
-      <c r="C26" s="22"/>
+      <c r="C26" s="9"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="10"/>
@@ -927,7 +920,7 @@
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="8"/>
       <c r="B28" s="9"/>
-      <c r="C28" s="22"/>
+      <c r="C28" s="9"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="10"/>
@@ -937,7 +930,7 @@
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="8"/>
       <c r="B30" s="9"/>
-      <c r="C30" s="22"/>
+      <c r="C30" s="9"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="10"/>
@@ -947,7 +940,7 @@
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="8"/>
       <c r="B32" s="9"/>
-      <c r="C32" s="22"/>
+      <c r="C32" s="9"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="10"/>
@@ -957,7 +950,7 @@
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="8"/>
       <c r="B34" s="9"/>
-      <c r="C34" s="22"/>
+      <c r="C34" s="9"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="10"/>
@@ -967,7 +960,7 @@
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="8"/>
       <c r="B36" s="9"/>
-      <c r="C36" s="22"/>
+      <c r="C36" s="9"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="10"/>
@@ -977,7 +970,7 @@
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="8"/>
       <c r="B38" s="9"/>
-      <c r="C38" s="22"/>
+      <c r="C38" s="9"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="10"/>
@@ -987,7 +980,7 @@
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="8"/>
       <c r="B40" s="9"/>
-      <c r="C40" s="22"/>
+      <c r="C40" s="9"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="10"/>
@@ -997,7 +990,7 @@
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="8"/>
       <c r="B42" s="9"/>
-      <c r="C42" s="22"/>
+      <c r="C42" s="9"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="10"/>
@@ -1007,7 +1000,7 @@
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="8"/>
       <c r="B44" s="9"/>
-      <c r="C44" s="22"/>
+      <c r="C44" s="9"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="10"/>
@@ -1017,7 +1010,7 @@
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="8"/>
       <c r="B46" s="9"/>
-      <c r="C46" s="22"/>
+      <c r="C46" s="9"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="10"/>
@@ -1027,7 +1020,7 @@
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="8"/>
       <c r="B48" s="9"/>
-      <c r="C48" s="22"/>
+      <c r="C48" s="9"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="10"/>
@@ -1037,7 +1030,7 @@
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="8"/>
       <c r="B50" s="9"/>
-      <c r="C50" s="22"/>
+      <c r="C50" s="9"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="6"/>
@@ -1047,7 +1040,7 @@
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="8"/>
       <c r="B52" s="9"/>
-      <c r="C52" s="22"/>
+      <c r="C52" s="9"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="6"/>
@@ -1057,7 +1050,7 @@
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="8"/>
       <c r="B54" s="9"/>
-      <c r="C54" s="22"/>
+      <c r="C54" s="9"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="6"/>
@@ -1067,7 +1060,7 @@
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="8"/>
       <c r="B56" s="9"/>
-      <c r="C56" s="22"/>
+      <c r="C56" s="9"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="6"/>
@@ -1077,7 +1070,7 @@
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="8"/>
       <c r="B58" s="9"/>
-      <c r="C58" s="22"/>
+      <c r="C58" s="9"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="6"/>
@@ -1087,7 +1080,7 @@
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="8"/>
       <c r="B60" s="9"/>
-      <c r="C60" s="22"/>
+      <c r="C60" s="9"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="6"/>
@@ -1097,7 +1090,7 @@
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="8"/>
       <c r="B62" s="9"/>
-      <c r="C62" s="22"/>
+      <c r="C62" s="9"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="6"/>
@@ -1107,7 +1100,7 @@
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="8"/>
       <c r="B64" s="9"/>
-      <c r="C64" s="22"/>
+      <c r="C64" s="9"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="6"/>
@@ -1117,7 +1110,7 @@
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="8"/>
       <c r="B66" s="9"/>
-      <c r="C66" s="22"/>
+      <c r="C66" s="9"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="6"/>
@@ -1127,7 +1120,7 @@
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="8"/>
       <c r="B68" s="9"/>
-      <c r="C68" s="22"/>
+      <c r="C68" s="9"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="6"/>
@@ -1137,7 +1130,7 @@
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="8"/>
       <c r="B70" s="9"/>
-      <c r="C70" s="22"/>
+      <c r="C70" s="9"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="6"/>
@@ -1147,7 +1140,7 @@
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="8"/>
       <c r="B72" s="9"/>
-      <c r="C72" s="22"/>
+      <c r="C72" s="9"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="6"/>
@@ -1157,7 +1150,7 @@
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="8"/>
       <c r="B74" s="9"/>
-      <c r="C74" s="22"/>
+      <c r="C74" s="9"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="6"/>
@@ -1167,7 +1160,7 @@
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="8"/>
       <c r="B76" s="9"/>
-      <c r="C76" s="22"/>
+      <c r="C76" s="9"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="6"/>
@@ -1177,7 +1170,7 @@
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="8"/>
       <c r="B78" s="9"/>
-      <c r="C78" s="22"/>
+      <c r="C78" s="9"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="6"/>
@@ -1187,7 +1180,7 @@
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="8"/>
       <c r="B80" s="9"/>
-      <c r="C80" s="22"/>
+      <c r="C80" s="9"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="6"/>
@@ -1197,7 +1190,7 @@
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="8"/>
       <c r="B82" s="9"/>
-      <c r="C82" s="22"/>
+      <c r="C82" s="9"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="6"/>
@@ -1207,7 +1200,7 @@
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="8"/>
       <c r="B84" s="9"/>
-      <c r="C84" s="22"/>
+      <c r="C84" s="9"/>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="6"/>
@@ -1217,7 +1210,7 @@
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="8"/>
       <c r="B86" s="9"/>
-      <c r="C86" s="22"/>
+      <c r="C86" s="9"/>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="6"/>
@@ -1227,7 +1220,7 @@
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="8"/>
       <c r="B88" s="9"/>
-      <c r="C88" s="22"/>
+      <c r="C88" s="9"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="6"/>
@@ -1237,7 +1230,7 @@
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="8"/>
       <c r="B90" s="9"/>
-      <c r="C90" s="22"/>
+      <c r="C90" s="9"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="6"/>
@@ -1247,7 +1240,7 @@
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="8"/>
       <c r="B92" s="9"/>
-      <c r="C92" s="22"/>
+      <c r="C92" s="9"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="6"/>
@@ -1257,7 +1250,7 @@
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="8"/>
       <c r="B94" s="9"/>
-      <c r="C94" s="22"/>
+      <c r="C94" s="9"/>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="6"/>
@@ -1267,7 +1260,7 @@
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="8"/>
       <c r="B96" s="9"/>
-      <c r="C96" s="22"/>
+      <c r="C96" s="9"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="6"/>
@@ -1277,7 +1270,7 @@
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="8"/>
       <c r="B98" s="9"/>
-      <c r="C98" s="22"/>
+      <c r="C98" s="9"/>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="6"/>
@@ -1287,7 +1280,7 @@
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="8"/>
       <c r="B100" s="9"/>
-      <c r="C100" s="22"/>
+      <c r="C100" s="9"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="6"/>
@@ -1297,7 +1290,7 @@
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="8"/>
       <c r="B102" s="9"/>
-      <c r="C102" s="22"/>
+      <c r="C102" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1308,7 +1301,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{175F71C0-CCE8-034C-8D7C-791DB0178004}">
           <x14:formula1>
-            <xm:f>Data!$C$2:$C$5</xm:f>
+            <xm:f>Data!$C$2:$C$4</xm:f>
           </x14:formula1>
           <xm:sqref>A3:A102</xm:sqref>
         </x14:dataValidation>
@@ -1342,7 +1335,7 @@
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.2">
@@ -1357,7 +1350,7 @@
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.2">
@@ -1419,9 +1412,6 @@
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="14" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -1432,7 +1422,7 @@
       <c r="A7" s="4"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="rnR3B9faacWpLg/dZCjGdnC4QB1ODvZ+8vO2zeJbvIf7CHGd56x4uQDZvmHOaYPCv/0BX6bhNelhSGm2z4wICw==" saltValue="o2FYOTf893qn90wx8pp9zw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="wnNF8dq4EQlAY3bw6Oejp7mW6UNCmjFIQvL86ndQn11xSnojYGhb8UEkkCGgZQaueviKI+2rXi9ZBo9BcThcEw==" saltValue="j9JeVYPBr1R2l4bt0sisbA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Add PLUS_CD in logement_edd.xlsx
</commit_message>
<xml_diff>
--- a/static/files/logements_edd.xlsx
+++ b/static/files/logements_edd.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/apilos/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2707DDD9-7FCB-FD47-86AA-0F39F1CB4F79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E24E18-5D98-8649-A595-4DDFC2903CA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1240" yWindow="500" windowWidth="27560" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Ici quelques explications</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>(Numéro de lot des logements inscrits dans les actes de vente/propriété…)</t>
+  </si>
+  <si>
+    <t>PLUS_CD</t>
   </si>
 </sst>
 </file>
@@ -173,7 +176,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -208,19 +211,6 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -315,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -323,33 +313,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -755,46 +744,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="68" x14ac:dyDescent="0.2">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="19" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="10"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="21"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="20"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="21"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="20"/>
     </row>
     <row r="6" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -805,9 +794,9 @@
       <c r="K6" s="5"/>
     </row>
     <row r="7" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="A7" s="10"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="21"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="20"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -818,479 +807,479 @@
       <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="21"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="20"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="21"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="20"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="8"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="10"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="21"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="20"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="8"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="10"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="21"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="20"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="8"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="10"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="21"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="20"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="8"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="10"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="21"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="20"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="8"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="10"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="21"/>
+      <c r="A21" s="9"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="20"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="8"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="10"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="21"/>
+      <c r="A23" s="9"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="20"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="8"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
+      <c r="A24" s="7"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="10"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="21"/>
+      <c r="A25" s="9"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="20"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="8"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
+      <c r="A26" s="7"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="10"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="21"/>
+      <c r="A27" s="9"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="20"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="8"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
+      <c r="A28" s="7"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="10"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="21"/>
+      <c r="A29" s="9"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="20"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="8"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
+      <c r="A30" s="7"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="10"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="21"/>
+      <c r="A31" s="9"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="20"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="8"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
+      <c r="A32" s="7"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="10"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="21"/>
+      <c r="A33" s="9"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="20"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="8"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
+      <c r="A34" s="7"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="10"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="21"/>
+      <c r="A35" s="9"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="20"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="8"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
+      <c r="A36" s="7"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="10"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="21"/>
+      <c r="A37" s="9"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="20"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="8"/>
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
+      <c r="A38" s="7"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="10"/>
-      <c r="B39" s="11"/>
-      <c r="C39" s="21"/>
+      <c r="A39" s="9"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="20"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="8"/>
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
+      <c r="A40" s="7"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="10"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="21"/>
+      <c r="A41" s="9"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="20"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="8"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
+      <c r="A42" s="7"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="10"/>
-      <c r="B43" s="11"/>
-      <c r="C43" s="21"/>
+      <c r="A43" s="9"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="20"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="8"/>
-      <c r="B44" s="9"/>
-      <c r="C44" s="9"/>
+      <c r="A44" s="7"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="10"/>
-      <c r="B45" s="11"/>
-      <c r="C45" s="21"/>
+      <c r="A45" s="9"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="20"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="8"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
+      <c r="A46" s="7"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="10"/>
-      <c r="B47" s="11"/>
-      <c r="C47" s="21"/>
+      <c r="A47" s="9"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="20"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="8"/>
-      <c r="B48" s="9"/>
-      <c r="C48" s="9"/>
+      <c r="A48" s="7"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="10"/>
-      <c r="B49" s="11"/>
-      <c r="C49" s="21"/>
+      <c r="A49" s="9"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="20"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="8"/>
-      <c r="B50" s="9"/>
-      <c r="C50" s="9"/>
+      <c r="A50" s="7"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="6"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="21"/>
+      <c r="A51" s="9"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="20"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="8"/>
-      <c r="B52" s="9"/>
-      <c r="C52" s="9"/>
+      <c r="A52" s="7"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="6"/>
-      <c r="B53" s="7"/>
-      <c r="C53" s="21"/>
+      <c r="A53" s="9"/>
+      <c r="B53" s="6"/>
+      <c r="C53" s="20"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="8"/>
-      <c r="B54" s="9"/>
-      <c r="C54" s="9"/>
+      <c r="A54" s="7"/>
+      <c r="B54" s="8"/>
+      <c r="C54" s="8"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="6"/>
-      <c r="B55" s="7"/>
-      <c r="C55" s="21"/>
+      <c r="A55" s="9"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="20"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="8"/>
-      <c r="B56" s="9"/>
-      <c r="C56" s="9"/>
+      <c r="A56" s="7"/>
+      <c r="B56" s="8"/>
+      <c r="C56" s="8"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="6"/>
-      <c r="B57" s="7"/>
-      <c r="C57" s="21"/>
+      <c r="A57" s="9"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="20"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="8"/>
-      <c r="B58" s="9"/>
-      <c r="C58" s="9"/>
+      <c r="A58" s="7"/>
+      <c r="B58" s="8"/>
+      <c r="C58" s="8"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="6"/>
-      <c r="B59" s="7"/>
-      <c r="C59" s="21"/>
+      <c r="A59" s="9"/>
+      <c r="B59" s="6"/>
+      <c r="C59" s="20"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" s="8"/>
-      <c r="B60" s="9"/>
-      <c r="C60" s="9"/>
+      <c r="A60" s="7"/>
+      <c r="B60" s="8"/>
+      <c r="C60" s="8"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" s="6"/>
-      <c r="B61" s="7"/>
-      <c r="C61" s="21"/>
+      <c r="A61" s="9"/>
+      <c r="B61" s="6"/>
+      <c r="C61" s="20"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="8"/>
-      <c r="B62" s="9"/>
-      <c r="C62" s="9"/>
+      <c r="A62" s="7"/>
+      <c r="B62" s="8"/>
+      <c r="C62" s="8"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="6"/>
-      <c r="B63" s="7"/>
-      <c r="C63" s="21"/>
+      <c r="A63" s="9"/>
+      <c r="B63" s="6"/>
+      <c r="C63" s="20"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" s="8"/>
-      <c r="B64" s="9"/>
-      <c r="C64" s="9"/>
+      <c r="A64" s="7"/>
+      <c r="B64" s="8"/>
+      <c r="C64" s="8"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" s="6"/>
-      <c r="B65" s="7"/>
-      <c r="C65" s="21"/>
+      <c r="A65" s="9"/>
+      <c r="B65" s="6"/>
+      <c r="C65" s="20"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" s="8"/>
-      <c r="B66" s="9"/>
-      <c r="C66" s="9"/>
+      <c r="A66" s="7"/>
+      <c r="B66" s="8"/>
+      <c r="C66" s="8"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="6"/>
-      <c r="B67" s="7"/>
-      <c r="C67" s="21"/>
+      <c r="A67" s="9"/>
+      <c r="B67" s="6"/>
+      <c r="C67" s="20"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="8"/>
-      <c r="B68" s="9"/>
-      <c r="C68" s="9"/>
+      <c r="A68" s="7"/>
+      <c r="B68" s="8"/>
+      <c r="C68" s="8"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" s="6"/>
-      <c r="B69" s="7"/>
-      <c r="C69" s="21"/>
+      <c r="A69" s="9"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="20"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="8"/>
-      <c r="B70" s="9"/>
-      <c r="C70" s="9"/>
+      <c r="A70" s="7"/>
+      <c r="B70" s="8"/>
+      <c r="C70" s="8"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" s="6"/>
-      <c r="B71" s="7"/>
-      <c r="C71" s="21"/>
+      <c r="A71" s="9"/>
+      <c r="B71" s="6"/>
+      <c r="C71" s="20"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" s="8"/>
-      <c r="B72" s="9"/>
-      <c r="C72" s="9"/>
+      <c r="A72" s="7"/>
+      <c r="B72" s="8"/>
+      <c r="C72" s="8"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" s="6"/>
-      <c r="B73" s="7"/>
-      <c r="C73" s="21"/>
+      <c r="A73" s="9"/>
+      <c r="B73" s="6"/>
+      <c r="C73" s="20"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" s="8"/>
-      <c r="B74" s="9"/>
-      <c r="C74" s="9"/>
+      <c r="A74" s="7"/>
+      <c r="B74" s="8"/>
+      <c r="C74" s="8"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75" s="6"/>
-      <c r="B75" s="7"/>
-      <c r="C75" s="21"/>
+      <c r="A75" s="9"/>
+      <c r="B75" s="6"/>
+      <c r="C75" s="20"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76" s="8"/>
-      <c r="B76" s="9"/>
-      <c r="C76" s="9"/>
+      <c r="A76" s="7"/>
+      <c r="B76" s="8"/>
+      <c r="C76" s="8"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A77" s="6"/>
-      <c r="B77" s="7"/>
-      <c r="C77" s="21"/>
+      <c r="A77" s="9"/>
+      <c r="B77" s="6"/>
+      <c r="C77" s="20"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78" s="8"/>
-      <c r="B78" s="9"/>
-      <c r="C78" s="9"/>
+      <c r="A78" s="7"/>
+      <c r="B78" s="8"/>
+      <c r="C78" s="8"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" s="6"/>
-      <c r="B79" s="7"/>
-      <c r="C79" s="21"/>
+      <c r="A79" s="9"/>
+      <c r="B79" s="6"/>
+      <c r="C79" s="20"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80" s="8"/>
-      <c r="B80" s="9"/>
-      <c r="C80" s="9"/>
+      <c r="A80" s="7"/>
+      <c r="B80" s="8"/>
+      <c r="C80" s="8"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" s="6"/>
-      <c r="B81" s="7"/>
-      <c r="C81" s="21"/>
+      <c r="A81" s="9"/>
+      <c r="B81" s="6"/>
+      <c r="C81" s="20"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" s="8"/>
-      <c r="B82" s="9"/>
-      <c r="C82" s="9"/>
+      <c r="A82" s="7"/>
+      <c r="B82" s="8"/>
+      <c r="C82" s="8"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A83" s="6"/>
-      <c r="B83" s="7"/>
-      <c r="C83" s="21"/>
+      <c r="A83" s="9"/>
+      <c r="B83" s="6"/>
+      <c r="C83" s="20"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84" s="8"/>
-      <c r="B84" s="9"/>
-      <c r="C84" s="9"/>
+      <c r="A84" s="7"/>
+      <c r="B84" s="8"/>
+      <c r="C84" s="8"/>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A85" s="6"/>
-      <c r="B85" s="7"/>
-      <c r="C85" s="21"/>
+      <c r="A85" s="9"/>
+      <c r="B85" s="6"/>
+      <c r="C85" s="20"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A86" s="8"/>
-      <c r="B86" s="9"/>
-      <c r="C86" s="9"/>
+      <c r="A86" s="7"/>
+      <c r="B86" s="8"/>
+      <c r="C86" s="8"/>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A87" s="6"/>
-      <c r="B87" s="7"/>
-      <c r="C87" s="21"/>
+      <c r="A87" s="9"/>
+      <c r="B87" s="6"/>
+      <c r="C87" s="20"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A88" s="8"/>
-      <c r="B88" s="9"/>
-      <c r="C88" s="9"/>
+      <c r="A88" s="7"/>
+      <c r="B88" s="8"/>
+      <c r="C88" s="8"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A89" s="6"/>
-      <c r="B89" s="7"/>
-      <c r="C89" s="21"/>
+      <c r="A89" s="9"/>
+      <c r="B89" s="6"/>
+      <c r="C89" s="20"/>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A90" s="8"/>
-      <c r="B90" s="9"/>
-      <c r="C90" s="9"/>
+      <c r="A90" s="7"/>
+      <c r="B90" s="8"/>
+      <c r="C90" s="8"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A91" s="6"/>
-      <c r="B91" s="7"/>
-      <c r="C91" s="21"/>
+      <c r="A91" s="9"/>
+      <c r="B91" s="6"/>
+      <c r="C91" s="20"/>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A92" s="8"/>
-      <c r="B92" s="9"/>
-      <c r="C92" s="9"/>
+      <c r="A92" s="7"/>
+      <c r="B92" s="8"/>
+      <c r="C92" s="8"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A93" s="6"/>
-      <c r="B93" s="7"/>
-      <c r="C93" s="21"/>
+      <c r="A93" s="9"/>
+      <c r="B93" s="6"/>
+      <c r="C93" s="20"/>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A94" s="8"/>
-      <c r="B94" s="9"/>
-      <c r="C94" s="9"/>
+      <c r="A94" s="7"/>
+      <c r="B94" s="8"/>
+      <c r="C94" s="8"/>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A95" s="6"/>
-      <c r="B95" s="7"/>
-      <c r="C95" s="21"/>
+      <c r="A95" s="9"/>
+      <c r="B95" s="6"/>
+      <c r="C95" s="20"/>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A96" s="8"/>
-      <c r="B96" s="9"/>
-      <c r="C96" s="9"/>
+      <c r="A96" s="7"/>
+      <c r="B96" s="8"/>
+      <c r="C96" s="8"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A97" s="6"/>
-      <c r="B97" s="7"/>
-      <c r="C97" s="21"/>
+      <c r="A97" s="9"/>
+      <c r="B97" s="6"/>
+      <c r="C97" s="20"/>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A98" s="8"/>
-      <c r="B98" s="9"/>
-      <c r="C98" s="9"/>
+      <c r="A98" s="7"/>
+      <c r="B98" s="8"/>
+      <c r="C98" s="8"/>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A99" s="6"/>
-      <c r="B99" s="7"/>
-      <c r="C99" s="21"/>
+      <c r="A99" s="9"/>
+      <c r="B99" s="6"/>
+      <c r="C99" s="20"/>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A100" s="8"/>
-      <c r="B100" s="9"/>
-      <c r="C100" s="9"/>
+      <c r="A100" s="7"/>
+      <c r="B100" s="8"/>
+      <c r="C100" s="8"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A101" s="6"/>
-      <c r="B101" s="7"/>
-      <c r="C101" s="21"/>
+      <c r="A101" s="9"/>
+      <c r="B101" s="6"/>
+      <c r="C101" s="20"/>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A102" s="8"/>
-      <c r="B102" s="9"/>
-      <c r="C102" s="9"/>
+      <c r="A102" s="7"/>
+      <c r="B102" s="8"/>
+      <c r="C102" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1299,9 +1288,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{175F71C0-CCE8-034C-8D7C-791DB0178004}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{59EB41A3-BA45-9F4B-B657-D354362CDCE4}">
           <x14:formula1>
-            <xm:f>Data!$C$2:$C$4</xm:f>
+            <xm:f>Data!$C$2:$C$5</xm:f>
           </x14:formula1>
           <xm:sqref>A3:A102</xm:sqref>
         </x14:dataValidation>
@@ -1368,7 +1357,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4880C39C-0BD9-B447-909B-7F37D33CA805}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1380,7 +1371,7 @@
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1388,7 +1379,7 @@
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1396,7 +1387,7 @@
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1404,7 +1395,7 @@
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1412,6 +1403,9 @@
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="C5" s="13" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -1422,7 +1416,7 @@
       <c r="A7" s="4"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="wnNF8dq4EQlAY3bw6Oejp7mW6UNCmjFIQvL86ndQn11xSnojYGhb8UEkkCGgZQaueviKI+2rXi9ZBo9BcThcEw==" saltValue="j9JeVYPBr1R2l4bt0sisbA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="G7XyjjW09t23q0x1IFSfKMTjj6pKjHfG4OzwwIrlaKDR0u0ZnLj2PyP05K91h9VA+TbErXRoN/jN0B3zfkQJ6A==" saltValue="crgplngORk/3Jem/pRh4AA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Add financement PLUS_CD same as PLUS (#1044)
* Add PLUS_CD as available financement

* Add PLUS_CD in logement_edd.xlsx

* fix and add tests

* Add missing migrations
</commit_message>
<xml_diff>
--- a/static/files/logements_edd.xlsx
+++ b/static/files/logements_edd.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/apilos/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2707DDD9-7FCB-FD47-86AA-0F39F1CB4F79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E24E18-5D98-8649-A595-4DDFC2903CA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1240" yWindow="500" windowWidth="27560" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Ici quelques explications</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>(Numéro de lot des logements inscrits dans les actes de vente/propriété…)</t>
+  </si>
+  <si>
+    <t>PLUS_CD</t>
   </si>
 </sst>
 </file>
@@ -173,7 +176,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -208,19 +211,6 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -315,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -323,33 +313,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -755,46 +744,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="68" x14ac:dyDescent="0.2">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="19" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="10"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="21"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="20"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="21"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="20"/>
     </row>
     <row r="6" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -805,9 +794,9 @@
       <c r="K6" s="5"/>
     </row>
     <row r="7" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="A7" s="10"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="21"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="20"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -818,479 +807,479 @@
       <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="21"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="20"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="21"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="20"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="8"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="10"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="21"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="20"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="8"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="10"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="21"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="20"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="8"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="10"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="21"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="20"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="8"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="10"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="21"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="20"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="8"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="10"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="21"/>
+      <c r="A21" s="9"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="20"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="8"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="10"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="21"/>
+      <c r="A23" s="9"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="20"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="8"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
+      <c r="A24" s="7"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="10"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="21"/>
+      <c r="A25" s="9"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="20"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="8"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
+      <c r="A26" s="7"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="10"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="21"/>
+      <c r="A27" s="9"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="20"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="8"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
+      <c r="A28" s="7"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="10"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="21"/>
+      <c r="A29" s="9"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="20"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="8"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
+      <c r="A30" s="7"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="10"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="21"/>
+      <c r="A31" s="9"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="20"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="8"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
+      <c r="A32" s="7"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="10"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="21"/>
+      <c r="A33" s="9"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="20"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="8"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
+      <c r="A34" s="7"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="10"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="21"/>
+      <c r="A35" s="9"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="20"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="8"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
+      <c r="A36" s="7"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="10"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="21"/>
+      <c r="A37" s="9"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="20"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="8"/>
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
+      <c r="A38" s="7"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="10"/>
-      <c r="B39" s="11"/>
-      <c r="C39" s="21"/>
+      <c r="A39" s="9"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="20"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="8"/>
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
+      <c r="A40" s="7"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="10"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="21"/>
+      <c r="A41" s="9"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="20"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="8"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
+      <c r="A42" s="7"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="10"/>
-      <c r="B43" s="11"/>
-      <c r="C43" s="21"/>
+      <c r="A43" s="9"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="20"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="8"/>
-      <c r="B44" s="9"/>
-      <c r="C44" s="9"/>
+      <c r="A44" s="7"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="10"/>
-      <c r="B45" s="11"/>
-      <c r="C45" s="21"/>
+      <c r="A45" s="9"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="20"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="8"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
+      <c r="A46" s="7"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="10"/>
-      <c r="B47" s="11"/>
-      <c r="C47" s="21"/>
+      <c r="A47" s="9"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="20"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="8"/>
-      <c r="B48" s="9"/>
-      <c r="C48" s="9"/>
+      <c r="A48" s="7"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="10"/>
-      <c r="B49" s="11"/>
-      <c r="C49" s="21"/>
+      <c r="A49" s="9"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="20"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="8"/>
-      <c r="B50" s="9"/>
-      <c r="C50" s="9"/>
+      <c r="A50" s="7"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="6"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="21"/>
+      <c r="A51" s="9"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="20"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="8"/>
-      <c r="B52" s="9"/>
-      <c r="C52" s="9"/>
+      <c r="A52" s="7"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="6"/>
-      <c r="B53" s="7"/>
-      <c r="C53" s="21"/>
+      <c r="A53" s="9"/>
+      <c r="B53" s="6"/>
+      <c r="C53" s="20"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="8"/>
-      <c r="B54" s="9"/>
-      <c r="C54" s="9"/>
+      <c r="A54" s="7"/>
+      <c r="B54" s="8"/>
+      <c r="C54" s="8"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="6"/>
-      <c r="B55" s="7"/>
-      <c r="C55" s="21"/>
+      <c r="A55" s="9"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="20"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="8"/>
-      <c r="B56" s="9"/>
-      <c r="C56" s="9"/>
+      <c r="A56" s="7"/>
+      <c r="B56" s="8"/>
+      <c r="C56" s="8"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="6"/>
-      <c r="B57" s="7"/>
-      <c r="C57" s="21"/>
+      <c r="A57" s="9"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="20"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="8"/>
-      <c r="B58" s="9"/>
-      <c r="C58" s="9"/>
+      <c r="A58" s="7"/>
+      <c r="B58" s="8"/>
+      <c r="C58" s="8"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="6"/>
-      <c r="B59" s="7"/>
-      <c r="C59" s="21"/>
+      <c r="A59" s="9"/>
+      <c r="B59" s="6"/>
+      <c r="C59" s="20"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" s="8"/>
-      <c r="B60" s="9"/>
-      <c r="C60" s="9"/>
+      <c r="A60" s="7"/>
+      <c r="B60" s="8"/>
+      <c r="C60" s="8"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" s="6"/>
-      <c r="B61" s="7"/>
-      <c r="C61" s="21"/>
+      <c r="A61" s="9"/>
+      <c r="B61" s="6"/>
+      <c r="C61" s="20"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="8"/>
-      <c r="B62" s="9"/>
-      <c r="C62" s="9"/>
+      <c r="A62" s="7"/>
+      <c r="B62" s="8"/>
+      <c r="C62" s="8"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="6"/>
-      <c r="B63" s="7"/>
-      <c r="C63" s="21"/>
+      <c r="A63" s="9"/>
+      <c r="B63" s="6"/>
+      <c r="C63" s="20"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" s="8"/>
-      <c r="B64" s="9"/>
-      <c r="C64" s="9"/>
+      <c r="A64" s="7"/>
+      <c r="B64" s="8"/>
+      <c r="C64" s="8"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" s="6"/>
-      <c r="B65" s="7"/>
-      <c r="C65" s="21"/>
+      <c r="A65" s="9"/>
+      <c r="B65" s="6"/>
+      <c r="C65" s="20"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" s="8"/>
-      <c r="B66" s="9"/>
-      <c r="C66" s="9"/>
+      <c r="A66" s="7"/>
+      <c r="B66" s="8"/>
+      <c r="C66" s="8"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="6"/>
-      <c r="B67" s="7"/>
-      <c r="C67" s="21"/>
+      <c r="A67" s="9"/>
+      <c r="B67" s="6"/>
+      <c r="C67" s="20"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="8"/>
-      <c r="B68" s="9"/>
-      <c r="C68" s="9"/>
+      <c r="A68" s="7"/>
+      <c r="B68" s="8"/>
+      <c r="C68" s="8"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" s="6"/>
-      <c r="B69" s="7"/>
-      <c r="C69" s="21"/>
+      <c r="A69" s="9"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="20"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="8"/>
-      <c r="B70" s="9"/>
-      <c r="C70" s="9"/>
+      <c r="A70" s="7"/>
+      <c r="B70" s="8"/>
+      <c r="C70" s="8"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" s="6"/>
-      <c r="B71" s="7"/>
-      <c r="C71" s="21"/>
+      <c r="A71" s="9"/>
+      <c r="B71" s="6"/>
+      <c r="C71" s="20"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" s="8"/>
-      <c r="B72" s="9"/>
-      <c r="C72" s="9"/>
+      <c r="A72" s="7"/>
+      <c r="B72" s="8"/>
+      <c r="C72" s="8"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" s="6"/>
-      <c r="B73" s="7"/>
-      <c r="C73" s="21"/>
+      <c r="A73" s="9"/>
+      <c r="B73" s="6"/>
+      <c r="C73" s="20"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" s="8"/>
-      <c r="B74" s="9"/>
-      <c r="C74" s="9"/>
+      <c r="A74" s="7"/>
+      <c r="B74" s="8"/>
+      <c r="C74" s="8"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75" s="6"/>
-      <c r="B75" s="7"/>
-      <c r="C75" s="21"/>
+      <c r="A75" s="9"/>
+      <c r="B75" s="6"/>
+      <c r="C75" s="20"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76" s="8"/>
-      <c r="B76" s="9"/>
-      <c r="C76" s="9"/>
+      <c r="A76" s="7"/>
+      <c r="B76" s="8"/>
+      <c r="C76" s="8"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A77" s="6"/>
-      <c r="B77" s="7"/>
-      <c r="C77" s="21"/>
+      <c r="A77" s="9"/>
+      <c r="B77" s="6"/>
+      <c r="C77" s="20"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78" s="8"/>
-      <c r="B78" s="9"/>
-      <c r="C78" s="9"/>
+      <c r="A78" s="7"/>
+      <c r="B78" s="8"/>
+      <c r="C78" s="8"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" s="6"/>
-      <c r="B79" s="7"/>
-      <c r="C79" s="21"/>
+      <c r="A79" s="9"/>
+      <c r="B79" s="6"/>
+      <c r="C79" s="20"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80" s="8"/>
-      <c r="B80" s="9"/>
-      <c r="C80" s="9"/>
+      <c r="A80" s="7"/>
+      <c r="B80" s="8"/>
+      <c r="C80" s="8"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" s="6"/>
-      <c r="B81" s="7"/>
-      <c r="C81" s="21"/>
+      <c r="A81" s="9"/>
+      <c r="B81" s="6"/>
+      <c r="C81" s="20"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" s="8"/>
-      <c r="B82" s="9"/>
-      <c r="C82" s="9"/>
+      <c r="A82" s="7"/>
+      <c r="B82" s="8"/>
+      <c r="C82" s="8"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A83" s="6"/>
-      <c r="B83" s="7"/>
-      <c r="C83" s="21"/>
+      <c r="A83" s="9"/>
+      <c r="B83" s="6"/>
+      <c r="C83" s="20"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84" s="8"/>
-      <c r="B84" s="9"/>
-      <c r="C84" s="9"/>
+      <c r="A84" s="7"/>
+      <c r="B84" s="8"/>
+      <c r="C84" s="8"/>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A85" s="6"/>
-      <c r="B85" s="7"/>
-      <c r="C85" s="21"/>
+      <c r="A85" s="9"/>
+      <c r="B85" s="6"/>
+      <c r="C85" s="20"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A86" s="8"/>
-      <c r="B86" s="9"/>
-      <c r="C86" s="9"/>
+      <c r="A86" s="7"/>
+      <c r="B86" s="8"/>
+      <c r="C86" s="8"/>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A87" s="6"/>
-      <c r="B87" s="7"/>
-      <c r="C87" s="21"/>
+      <c r="A87" s="9"/>
+      <c r="B87" s="6"/>
+      <c r="C87" s="20"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A88" s="8"/>
-      <c r="B88" s="9"/>
-      <c r="C88" s="9"/>
+      <c r="A88" s="7"/>
+      <c r="B88" s="8"/>
+      <c r="C88" s="8"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A89" s="6"/>
-      <c r="B89" s="7"/>
-      <c r="C89" s="21"/>
+      <c r="A89" s="9"/>
+      <c r="B89" s="6"/>
+      <c r="C89" s="20"/>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A90" s="8"/>
-      <c r="B90" s="9"/>
-      <c r="C90" s="9"/>
+      <c r="A90" s="7"/>
+      <c r="B90" s="8"/>
+      <c r="C90" s="8"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A91" s="6"/>
-      <c r="B91" s="7"/>
-      <c r="C91" s="21"/>
+      <c r="A91" s="9"/>
+      <c r="B91" s="6"/>
+      <c r="C91" s="20"/>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A92" s="8"/>
-      <c r="B92" s="9"/>
-      <c r="C92" s="9"/>
+      <c r="A92" s="7"/>
+      <c r="B92" s="8"/>
+      <c r="C92" s="8"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A93" s="6"/>
-      <c r="B93" s="7"/>
-      <c r="C93" s="21"/>
+      <c r="A93" s="9"/>
+      <c r="B93" s="6"/>
+      <c r="C93" s="20"/>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A94" s="8"/>
-      <c r="B94" s="9"/>
-      <c r="C94" s="9"/>
+      <c r="A94" s="7"/>
+      <c r="B94" s="8"/>
+      <c r="C94" s="8"/>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A95" s="6"/>
-      <c r="B95" s="7"/>
-      <c r="C95" s="21"/>
+      <c r="A95" s="9"/>
+      <c r="B95" s="6"/>
+      <c r="C95" s="20"/>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A96" s="8"/>
-      <c r="B96" s="9"/>
-      <c r="C96" s="9"/>
+      <c r="A96" s="7"/>
+      <c r="B96" s="8"/>
+      <c r="C96" s="8"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A97" s="6"/>
-      <c r="B97" s="7"/>
-      <c r="C97" s="21"/>
+      <c r="A97" s="9"/>
+      <c r="B97" s="6"/>
+      <c r="C97" s="20"/>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A98" s="8"/>
-      <c r="B98" s="9"/>
-      <c r="C98" s="9"/>
+      <c r="A98" s="7"/>
+      <c r="B98" s="8"/>
+      <c r="C98" s="8"/>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A99" s="6"/>
-      <c r="B99" s="7"/>
-      <c r="C99" s="21"/>
+      <c r="A99" s="9"/>
+      <c r="B99" s="6"/>
+      <c r="C99" s="20"/>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A100" s="8"/>
-      <c r="B100" s="9"/>
-      <c r="C100" s="9"/>
+      <c r="A100" s="7"/>
+      <c r="B100" s="8"/>
+      <c r="C100" s="8"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A101" s="6"/>
-      <c r="B101" s="7"/>
-      <c r="C101" s="21"/>
+      <c r="A101" s="9"/>
+      <c r="B101" s="6"/>
+      <c r="C101" s="20"/>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A102" s="8"/>
-      <c r="B102" s="9"/>
-      <c r="C102" s="9"/>
+      <c r="A102" s="7"/>
+      <c r="B102" s="8"/>
+      <c r="C102" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1299,9 +1288,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{175F71C0-CCE8-034C-8D7C-791DB0178004}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{59EB41A3-BA45-9F4B-B657-D354362CDCE4}">
           <x14:formula1>
-            <xm:f>Data!$C$2:$C$4</xm:f>
+            <xm:f>Data!$C$2:$C$5</xm:f>
           </x14:formula1>
           <xm:sqref>A3:A102</xm:sqref>
         </x14:dataValidation>
@@ -1368,7 +1357,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4880C39C-0BD9-B447-909B-7F37D33CA805}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1380,7 +1371,7 @@
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1388,7 +1379,7 @@
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1396,7 +1387,7 @@
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1404,7 +1395,7 @@
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1412,6 +1403,9 @@
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="C5" s="13" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -1422,7 +1416,7 @@
       <c r="A7" s="4"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="wnNF8dq4EQlAY3bw6Oejp7mW6UNCmjFIQvL86ndQn11xSnojYGhb8UEkkCGgZQaueviKI+2rXi9ZBo9BcThcEw==" saltValue="j9JeVYPBr1R2l4bt0sisbA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="G7XyjjW09t23q0x1IFSfKMTjj6pKjHfG4OzwwIrlaKDR0u0ZnLj2PyP05K91h9VA+TbErXRoN/jN0B3zfkQJ6A==" saltValue="crgplngORk/3Jem/pRh4AA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>